<commit_message>
Update XLSX, build initial py script
</commit_message>
<xml_diff>
--- a/Research/TH9800_Packets.xlsx
+++ b/Research/TH9800_Packets.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SleepyNinja\.git\TH9800_CAT\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15099703-F812-45B8-BF3B-C2C0DE7C3B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590ED66-E1B7-4EB7-947C-36C51E901A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10910" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{96F0B5EF-7042-4BBD-B54F-B5D392DC829F}"/>
+    <workbookView xWindow="19090" yWindow="-10910" windowWidth="38620" windowHeight="21100" activeTab="7" xr2:uid="{96F0B5EF-7042-4BBD-B54F-B5D392DC829F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Power On Seq" sheetId="15" r:id="rId1"/>
-    <sheet name="Packets TX" sheetId="2" r:id="rId2"/>
-    <sheet name="AllPacketsTX" sheetId="3" r:id="rId3"/>
-    <sheet name="Checksum TX" sheetId="5" r:id="rId4"/>
-    <sheet name="RX NOTES" sheetId="16" r:id="rId5"/>
-    <sheet name="Packets RX" sheetId="6" r:id="rId6"/>
-    <sheet name="AllPacketsRX" sheetId="7" r:id="rId7"/>
-    <sheet name="RX_PWR_LVL" sheetId="10" r:id="rId8"/>
-    <sheet name="RX_V-M" sheetId="12" r:id="rId9"/>
-    <sheet name="TX when PTT" sheetId="18" r:id="rId10"/>
-    <sheet name="RX when PTT" sheetId="14" r:id="rId11"/>
-    <sheet name="Power Levels" sheetId="17" r:id="rId12"/>
-    <sheet name="STUN-REVIVE" sheetId="19" r:id="rId13"/>
+    <sheet name="Packets TX" sheetId="2" r:id="rId1"/>
+    <sheet name="AllPacketsTX" sheetId="3" r:id="rId2"/>
+    <sheet name="Checksum TX" sheetId="5" r:id="rId3"/>
+    <sheet name="RX NOTES" sheetId="16" r:id="rId4"/>
+    <sheet name="Packets RX" sheetId="6" r:id="rId5"/>
+    <sheet name="AllPacketsRX" sheetId="7" r:id="rId6"/>
+    <sheet name="RX_PWR_LVL" sheetId="10" r:id="rId7"/>
+    <sheet name="RX_V-M" sheetId="12" r:id="rId8"/>
+    <sheet name="TX when PTT" sheetId="18" r:id="rId9"/>
+    <sheet name="RX when PTT" sheetId="14" r:id="rId10"/>
+    <sheet name="Power Levels" sheetId="17" r:id="rId11"/>
+    <sheet name="STUN-REVIVE" sheetId="19" r:id="rId12"/>
+    <sheet name="Power On Seq" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3978" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3978" uniqueCount="523">
   <si>
     <t>0xAA</t>
   </si>
@@ -2275,6 +2275,12 @@
   <si>
     <t>35</t>
   </si>
+  <si>
+    <t>10 (or 12?)</t>
+  </si>
+  <si>
+    <t>02R (or 01L?)</t>
+  </si>
 </sst>
 </file>
 
@@ -2559,7 +2565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2672,24 +2678,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2714,11 +2702,23 @@
     <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3075,13 +3075,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
@@ -3090,6 +3083,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3137,7 +3137,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D80A179C-B31E-43C3-87C6-732FE1D9BAAC}" name="Table1" displayName="Table1" ref="A1:M70" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D80A179C-B31E-43C3-87C6-732FE1D9BAAC}" name="Table1" displayName="Table1" ref="A1:M70" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46">
   <autoFilter ref="A1:M70" xr:uid="{D80A179C-B31E-43C3-87C6-732FE1D9BAAC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M68">
     <sortCondition ref="E1:E68"/>
@@ -3477,2116 +3477,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15F8E68-08D0-4CAC-823D-87C2636A73EF}">
-  <dimension ref="B1:CV175"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F8))</f>
-        <v>AAFD018081</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" t="str" cm="1">
-        <f t="array" ref="F8:J8">TRANSPOSE(SUBSTITUTE(C4:C8,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G8" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H8" t="str">
-        <v>01</v>
-      </c>
-      <c r="I8" t="str">
-        <v>80</v>
-      </c>
-      <c r="J8" t="str">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F16))</f>
-        <v>AAFD02700072</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="F16" t="str" cm="1">
-        <f t="array" ref="F16:K16">TRANSPOSE(SUBSTITUTE(B11:B16,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G16" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H16" t="str">
-        <v>02</v>
-      </c>
-      <c r="I16" t="str">
-        <v>70</v>
-      </c>
-      <c r="J16" t="str">
-        <v>00</v>
-      </c>
-      <c r="K16" t="str">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F21" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F22))</f>
-        <v>AAFD01F0F1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" t="str" cm="1">
-        <f t="array" ref="F22:J22">TRANSPOSE(SUBSTITUTE(C18:C22,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G22" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H22" t="str">
-        <v>01</v>
-      </c>
-      <c r="I22" t="str">
-        <v>F0</v>
-      </c>
-      <c r="J22" t="str">
-        <v>F1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F29))</f>
-        <v>AAFD02720070</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="F29" t="str" cm="1">
-        <f t="array" ref="F29:K29">TRANSPOSE(SUBSTITUTE(B24:B29,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G29" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H29" t="str">
-        <v>02</v>
-      </c>
-      <c r="I29" t="str">
-        <v>72</v>
-      </c>
-      <c r="J29" t="str">
-        <v>00</v>
-      </c>
-      <c r="K29" t="str">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C33" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C35" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C36" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C40" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C41" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C43" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C44" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F46))</f>
-        <v>AAFD0C84FFFFFFFF01480002FF00003C</v>
-      </c>
-    </row>
-    <row r="46" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C46" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" t="str" cm="1">
-        <f t="array" ref="F46:U46">TRANSPOSE(SUBSTITUTE(C31:C46,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G46" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H46" t="str">
-        <v>0C</v>
-      </c>
-      <c r="I46" t="str">
-        <v>84</v>
-      </c>
-      <c r="J46" t="str">
-        <v>FF</v>
-      </c>
-      <c r="K46" t="str">
-        <v>FF</v>
-      </c>
-      <c r="L46" t="str">
-        <v>FF</v>
-      </c>
-      <c r="M46" t="str">
-        <v>FF</v>
-      </c>
-      <c r="N46" s="2" t="str">
-        <v>01</v>
-      </c>
-      <c r="O46" s="1" t="str">
-        <v>48</v>
-      </c>
-      <c r="P46" s="1" t="str">
-        <v>00</v>
-      </c>
-      <c r="Q46" s="1" t="str">
-        <v>02</v>
-      </c>
-      <c r="R46" t="str">
-        <v>FF</v>
-      </c>
-      <c r="S46" t="str">
-        <v>00</v>
-      </c>
-      <c r="T46" t="str">
-        <v>00</v>
-      </c>
-      <c r="U46" t="str">
-        <v>3C</v>
-      </c>
-    </row>
-    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C48" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C49" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C50" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C51" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C52" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C53" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C54" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C55" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C58" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C59" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C60" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="61" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C61" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F63))</f>
-        <v>AAFD0C84FFFFFFFF81220082A503000F</v>
-      </c>
-    </row>
-    <row r="63" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C63" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" t="str" cm="1">
-        <f t="array" ref="F63:U63">TRANSPOSE(SUBSTITUTE(C48:C63,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G63" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H63" t="str">
-        <v>0C</v>
-      </c>
-      <c r="I63" t="str">
-        <v>84</v>
-      </c>
-      <c r="J63" t="str">
-        <v>FF</v>
-      </c>
-      <c r="K63" t="str">
-        <v>FF</v>
-      </c>
-      <c r="L63" t="str">
-        <v>FF</v>
-      </c>
-      <c r="M63" t="str">
-        <v>FF</v>
-      </c>
-      <c r="N63" s="2" t="str">
-        <v>81</v>
-      </c>
-      <c r="O63" s="1" t="str">
-        <v>22</v>
-      </c>
-      <c r="P63" s="1" t="str">
-        <v>00</v>
-      </c>
-      <c r="Q63" s="1" t="str">
-        <v>82</v>
-      </c>
-      <c r="R63" t="str">
-        <v>A5</v>
-      </c>
-      <c r="S63" t="str">
-        <v>03</v>
-      </c>
-      <c r="T63" t="str">
-        <v>00</v>
-      </c>
-      <c r="U63" t="str">
-        <v>0F</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B65" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F70))</f>
-        <v>AAFD02522070</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B70" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="F70" t="str" cm="1">
-        <f t="array" ref="F70:K70">TRANSPOSE(SUBSTITUTE(B65:B70,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G70" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H70" t="str">
-        <v>02</v>
-      </c>
-      <c r="I70" t="str">
-        <v>52</v>
-      </c>
-      <c r="J70" t="str">
-        <v>20</v>
-      </c>
-      <c r="K70" t="str">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C72" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C75" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C77" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C78" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="F78" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F79))</f>
-        <v>AAFD03A01802B9</v>
-      </c>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E79" s="2"/>
-      <c r="F79" t="str" cm="1">
-        <f t="array" ref="F79:L79">TRANSPOSE(SUBSTITUTE(C72:C78,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G79" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H79" t="str">
-        <v>03</v>
-      </c>
-      <c r="I79" t="str">
-        <v>A0</v>
-      </c>
-      <c r="J79" t="str">
-        <v>18</v>
-      </c>
-      <c r="K79" t="str">
-        <v>02</v>
-      </c>
-      <c r="L79" t="str">
-        <v>B9</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="161" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B161" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="162" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B162" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="163" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B163" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="164" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B164" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B165" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B166" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="167" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B167" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="168" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B168" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="169" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B169" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="170" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B170" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B171" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B172" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="173" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B173" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="174" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B174" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F174" t="str">
-        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F175))</f>
-        <v>AAFD0341FF41FCAAFD02034342AAFD0602400020203175AAFD090140003253494D505825AAFD080440000080000008C4AAFD02030302AAFD0203C3C2AAFD0602C100334850EEAAFD0901C000203133315620ADAAFD0225C1E6AAFD02038382</v>
-      </c>
-    </row>
-    <row r="175" spans="2:100" x14ac:dyDescent="0.25">
-      <c r="B175" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F175" t="str" cm="1">
-        <f t="array" ref="F175:CV175">TRANSPOSE(SUBSTITUTE(B81:B175,"0x",""))</f>
-        <v>AA</v>
-      </c>
-      <c r="G175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="H175" t="str">
-        <v>03</v>
-      </c>
-      <c r="I175" t="str">
-        <v>41</v>
-      </c>
-      <c r="J175" t="str">
-        <v>FF</v>
-      </c>
-      <c r="K175" t="str">
-        <v>41</v>
-      </c>
-      <c r="L175" t="str">
-        <v>FC</v>
-      </c>
-      <c r="M175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="N175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="O175" t="str">
-        <v>02</v>
-      </c>
-      <c r="P175" t="str">
-        <v>03</v>
-      </c>
-      <c r="Q175" t="str">
-        <v>43</v>
-      </c>
-      <c r="R175" t="str">
-        <v>42</v>
-      </c>
-      <c r="S175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="T175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="U175" t="str">
-        <v>06</v>
-      </c>
-      <c r="V175" t="str">
-        <v>02</v>
-      </c>
-      <c r="W175" t="str">
-        <v>40</v>
-      </c>
-      <c r="X175" t="str">
-        <v>00</v>
-      </c>
-      <c r="Y175" t="str">
-        <v>20</v>
-      </c>
-      <c r="Z175" t="str">
-        <v>20</v>
-      </c>
-      <c r="AA175" t="str">
-        <v>31</v>
-      </c>
-      <c r="AB175" t="str">
-        <v>75</v>
-      </c>
-      <c r="AC175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="AD175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="AE175" t="str">
-        <v>09</v>
-      </c>
-      <c r="AF175" t="str">
-        <v>01</v>
-      </c>
-      <c r="AG175" t="str">
-        <v>40</v>
-      </c>
-      <c r="AH175" t="str">
-        <v>00</v>
-      </c>
-      <c r="AI175" t="str">
-        <v>32</v>
-      </c>
-      <c r="AJ175" t="str">
-        <v>53</v>
-      </c>
-      <c r="AK175" t="str">
-        <v>49</v>
-      </c>
-      <c r="AL175" t="str">
-        <v>4D</v>
-      </c>
-      <c r="AM175" t="str">
-        <v>50</v>
-      </c>
-      <c r="AN175" t="str">
-        <v>58</v>
-      </c>
-      <c r="AO175" t="str">
-        <v>25</v>
-      </c>
-      <c r="AP175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="AQ175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="AR175" t="str">
-        <v>08</v>
-      </c>
-      <c r="AS175" t="str">
-        <v>04</v>
-      </c>
-      <c r="AT175" t="str">
-        <v>40</v>
-      </c>
-      <c r="AU175" t="str">
-        <v>00</v>
-      </c>
-      <c r="AV175" t="str">
-        <v>00</v>
-      </c>
-      <c r="AW175" t="str">
-        <v>80</v>
-      </c>
-      <c r="AX175" t="str">
-        <v>00</v>
-      </c>
-      <c r="AY175" t="str">
-        <v>00</v>
-      </c>
-      <c r="AZ175" t="str">
-        <v>08</v>
-      </c>
-      <c r="BA175" t="str">
-        <v>C4</v>
-      </c>
-      <c r="BB175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="BC175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="BD175" t="str">
-        <v>02</v>
-      </c>
-      <c r="BE175" t="str">
-        <v>03</v>
-      </c>
-      <c r="BF175" t="str">
-        <v>03</v>
-      </c>
-      <c r="BG175" t="str">
-        <v>02</v>
-      </c>
-      <c r="BH175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="BI175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="BJ175" t="str">
-        <v>02</v>
-      </c>
-      <c r="BK175" t="str">
-        <v>03</v>
-      </c>
-      <c r="BL175" t="str">
-        <v>C3</v>
-      </c>
-      <c r="BM175" t="str">
-        <v>C2</v>
-      </c>
-      <c r="BN175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="BO175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="BP175" t="str">
-        <v>06</v>
-      </c>
-      <c r="BQ175" t="str">
-        <v>02</v>
-      </c>
-      <c r="BR175" t="str">
-        <v>C1</v>
-      </c>
-      <c r="BS175" t="str">
-        <v>00</v>
-      </c>
-      <c r="BT175" t="str">
-        <v>33</v>
-      </c>
-      <c r="BU175" t="str">
-        <v>48</v>
-      </c>
-      <c r="BV175" t="str">
-        <v>50</v>
-      </c>
-      <c r="BW175" t="str">
-        <v>EE</v>
-      </c>
-      <c r="BX175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="BY175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="BZ175" t="str">
-        <v>09</v>
-      </c>
-      <c r="CA175" t="str">
-        <v>01</v>
-      </c>
-      <c r="CB175" t="str">
-        <v>C0</v>
-      </c>
-      <c r="CC175" t="str">
-        <v>00</v>
-      </c>
-      <c r="CD175" t="str">
-        <v>20</v>
-      </c>
-      <c r="CE175" t="str">
-        <v>31</v>
-      </c>
-      <c r="CF175" t="str">
-        <v>33</v>
-      </c>
-      <c r="CG175" t="str">
-        <v>31</v>
-      </c>
-      <c r="CH175" t="str">
-        <v>56</v>
-      </c>
-      <c r="CI175" t="str">
-        <v>20</v>
-      </c>
-      <c r="CJ175" t="str">
-        <v>AD</v>
-      </c>
-      <c r="CK175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="CL175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="CM175" t="str">
-        <v>02</v>
-      </c>
-      <c r="CN175" t="str">
-        <v>25</v>
-      </c>
-      <c r="CO175" t="str">
-        <v>C1</v>
-      </c>
-      <c r="CP175" t="str">
-        <v>E6</v>
-      </c>
-      <c r="CQ175" t="str">
-        <v>AA</v>
-      </c>
-      <c r="CR175" t="str">
-        <v>FD</v>
-      </c>
-      <c r="CS175" t="str">
-        <v>02</v>
-      </c>
-      <c r="CT175" t="str">
-        <v>03</v>
-      </c>
-      <c r="CU175" t="str">
-        <v>83</v>
-      </c>
-      <c r="CV175" t="str">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:DD1048576">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
-      <formula>"AA"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
-      <formula>"FD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
-      <formula>"0xFD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
-      <formula>"0xAA"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF9E3CD-2759-404F-9723-870EF2ECB184}">
-  <dimension ref="A1:Z12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="20" customWidth="1"/>
-    <col min="7" max="26" width="9.140625" style="20"/>
-    <col min="27" max="16384" width="9.140625" style="41"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
-        <v>324</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="56" t="s">
-        <v>360</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1" s="58" t="s">
-        <v>292</v>
-      </c>
-      <c r="F1" s="59" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>487</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>326</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>340</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>490</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q2" s="61" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>338</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>369</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>315</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="H3" s="61" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>487</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>489</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>340</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>490</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>489</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q4" s="61" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>338</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>369</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>352</v>
-      </c>
-      <c r="G5" s="62" t="s">
-        <v>315</v>
-      </c>
-      <c r="H5" s="61" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
-        <v>486</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08C0377-036C-40B2-90AA-F809ED88AEF2}">
-  <dimension ref="B1:S23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I5" t="s">
-        <v>204</v>
-      </c>
-      <c r="J5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>5</v>
-      </c>
-      <c r="L10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="J11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L19" t="str" cm="1">
-        <f t="array" ref="L19">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(B2:B7)),"0x","")</f>
-        <v>AAFD021D031C</v>
-      </c>
-      <c r="M19" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="20" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L20" t="str" cm="1">
-        <f t="array" ref="L20">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(B8:B13)),"0x","")</f>
-        <v>AAFD02150116</v>
-      </c>
-      <c r="M20" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="21" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L21" t="str" cm="1">
-        <f t="array" ref="L21">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(C2:C7)),"0x","")</f>
-        <v>AAFD021D001F</v>
-      </c>
-      <c r="M21" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="22" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="L22" t="str" cm="1">
-        <f t="array" ref="L22">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(C8:C13)),"0x","")</f>
-        <v>AAFD02150017</v>
-      </c>
-      <c r="M22" t="s">
-        <v>308</v>
-      </c>
-      <c r="O22" t="str" cm="1">
-        <f t="array" ref="O22:S22">TRANSPOSE(B2:B6)</f>
-        <v>0xAA</v>
-      </c>
-      <c r="P22" t="str">
-        <v>0xFD</v>
-      </c>
-      <c r="Q22" t="str">
-        <v>0x02</v>
-      </c>
-      <c r="R22" t="str">
-        <v>0x1D</v>
-      </c>
-      <c r="S22" t="str">
-        <v>0x03</v>
-      </c>
-    </row>
-    <row r="23" spans="12:19" x14ac:dyDescent="0.25">
-      <c r="O23" t="str" cm="1">
-        <f t="array" ref="O23:S23">TRANSPOSE(B8:B12)</f>
-        <v>0xAA</v>
-      </c>
-      <c r="P23" t="str">
-        <v>0xFD</v>
-      </c>
-      <c r="Q23" t="str">
-        <v>0x02</v>
-      </c>
-      <c r="R23" t="str">
-        <v>0x15</v>
-      </c>
-      <c r="S23" t="str">
-        <v>0x01</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="G2:G13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"FD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"AA"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F427A6AF-1D90-4128-A669-92C981920ABE}">
-  <dimension ref="B1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S53" sqref="S53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
-        <v>422</v>
-      </c>
-      <c r="C2" s="51"/>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
-        <v>423</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
-        <v>424</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
-        <v>425</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="44" t="s">
-        <v>426</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD45E57-5088-4CDA-BA4B-E4E29697AAB7}">
-  <dimension ref="B2:F25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="122" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
-        <v>504</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F5" s="18" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
-        <v>508</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
-        <v>509</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F12" s="18" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F13" s="18" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="18" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
-        <v>485</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944D94CF-A2A0-4F25-9A9F-F93989AAC083}">
   <dimension ref="A1:AZ70"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:R20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5610,10 +3505,10 @@
       <c r="B1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="46"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="37" t="s">
         <v>291</v>
       </c>
@@ -5623,10 +3518,10 @@
       <c r="R1" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="U1" s="46"/>
+      <c r="U1" s="57"/>
       <c r="V1" s="37" t="s">
         <v>291</v>
       </c>
@@ -18562,12 +16457,1913 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08C0377-036C-40B2-90AA-F809ED88AEF2}">
+  <dimension ref="B1:S23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I5" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L19" t="str" cm="1">
+        <f t="array" ref="L19">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(B2:B7)),"0x","")</f>
+        <v>AAFD021D031C</v>
+      </c>
+      <c r="M19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L20" t="str" cm="1">
+        <f t="array" ref="L20">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(B8:B13)),"0x","")</f>
+        <v>AAFD02150116</v>
+      </c>
+      <c r="M20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="21" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L21" t="str" cm="1">
+        <f t="array" ref="L21">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(C2:C7)),"0x","")</f>
+        <v>AAFD021D001F</v>
+      </c>
+      <c r="M21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L22" t="str" cm="1">
+        <f t="array" ref="L22">SUBSTITUTE(TRANSPOSE(_xlfn.CONCAT(C8:C13)),"0x","")</f>
+        <v>AAFD02150017</v>
+      </c>
+      <c r="M22" t="s">
+        <v>308</v>
+      </c>
+      <c r="O22" t="str" cm="1">
+        <f t="array" ref="O22:S22">TRANSPOSE(B2:B6)</f>
+        <v>0xAA</v>
+      </c>
+      <c r="P22" t="str">
+        <v>0xFD</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>0x02</v>
+      </c>
+      <c r="R22" t="str">
+        <v>0x1D</v>
+      </c>
+      <c r="S22" t="str">
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="23" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="O23" t="str" cm="1">
+        <f t="array" ref="O23:S23">TRANSPOSE(B8:B12)</f>
+        <v>0xAA</v>
+      </c>
+      <c r="P23" t="str">
+        <v>0xFD</v>
+      </c>
+      <c r="Q23" t="str">
+        <v>0x02</v>
+      </c>
+      <c r="R23" t="str">
+        <v>0x15</v>
+      </c>
+      <c r="S23" t="str">
+        <v>0x01</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G13">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"FD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"AA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F427A6AF-1D90-4128-A669-92C981920ABE}">
+  <dimension ref="B1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S53" sqref="S53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="61" t="s">
+        <v>422</v>
+      </c>
+      <c r="C2" s="62"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="42" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="42" t="s">
+        <v>424</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>425</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="44" t="s">
+        <v>426</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD45E57-5088-4CDA-BA4B-E4E29697AAB7}">
+  <dimension ref="B2:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="122" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" s="18" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
+        <v>508</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" s="18" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="18" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>485</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15F8E68-08D0-4CAC-823D-87C2636A73EF}">
+  <dimension ref="B1:CV175"/>
+  <sheetViews>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F8))</f>
+        <v>AAFD018081</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" t="str" cm="1">
+        <f t="array" ref="F8:J8">TRANSPOSE(SUBSTITUTE(C4:C8,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G8" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H8" t="str">
+        <v>01</v>
+      </c>
+      <c r="I8" t="str">
+        <v>80</v>
+      </c>
+      <c r="J8" t="str">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F16))</f>
+        <v>AAFD02700072</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F16" t="str" cm="1">
+        <f t="array" ref="F16:K16">TRANSPOSE(SUBSTITUTE(B11:B16,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G16" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H16" t="str">
+        <v>02</v>
+      </c>
+      <c r="I16" t="str">
+        <v>70</v>
+      </c>
+      <c r="J16" t="str">
+        <v>00</v>
+      </c>
+      <c r="K16" t="str">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F21" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F22))</f>
+        <v>AAFD01F0F1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" t="str" cm="1">
+        <f t="array" ref="F22:J22">TRANSPOSE(SUBSTITUTE(C18:C22,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G22" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H22" t="str">
+        <v>01</v>
+      </c>
+      <c r="I22" t="str">
+        <v>F0</v>
+      </c>
+      <c r="J22" t="str">
+        <v>F1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F29))</f>
+        <v>AAFD02720070</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="F29" t="str" cm="1">
+        <f t="array" ref="F29:K29">TRANSPOSE(SUBSTITUTE(B24:B29,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G29" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H29" t="str">
+        <v>02</v>
+      </c>
+      <c r="I29" t="str">
+        <v>72</v>
+      </c>
+      <c r="J29" t="str">
+        <v>00</v>
+      </c>
+      <c r="K29" t="str">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F46))</f>
+        <v>AAFD0C84FFFFFFFF01480002FF00003C</v>
+      </c>
+    </row>
+    <row r="46" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C46" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" t="str" cm="1">
+        <f t="array" ref="F46:U46">TRANSPOSE(SUBSTITUTE(C31:C46,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G46" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H46" t="str">
+        <v>0C</v>
+      </c>
+      <c r="I46" t="str">
+        <v>84</v>
+      </c>
+      <c r="J46" t="str">
+        <v>FF</v>
+      </c>
+      <c r="K46" t="str">
+        <v>FF</v>
+      </c>
+      <c r="L46" t="str">
+        <v>FF</v>
+      </c>
+      <c r="M46" t="str">
+        <v>FF</v>
+      </c>
+      <c r="N46" s="2" t="str">
+        <v>01</v>
+      </c>
+      <c r="O46" s="1" t="str">
+        <v>48</v>
+      </c>
+      <c r="P46" s="1" t="str">
+        <v>00</v>
+      </c>
+      <c r="Q46" s="1" t="str">
+        <v>02</v>
+      </c>
+      <c r="R46" t="str">
+        <v>FF</v>
+      </c>
+      <c r="S46" t="str">
+        <v>00</v>
+      </c>
+      <c r="T46" t="str">
+        <v>00</v>
+      </c>
+      <c r="U46" t="str">
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C48" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C51" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C53" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C55" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C56" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C57" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C58" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C60" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C61" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F63))</f>
+        <v>AAFD0C84FFFFFFFF81220082A503000F</v>
+      </c>
+    </row>
+    <row r="63" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C63" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" t="str" cm="1">
+        <f t="array" ref="F63:U63">TRANSPOSE(SUBSTITUTE(C48:C63,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G63" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H63" t="str">
+        <v>0C</v>
+      </c>
+      <c r="I63" t="str">
+        <v>84</v>
+      </c>
+      <c r="J63" t="str">
+        <v>FF</v>
+      </c>
+      <c r="K63" t="str">
+        <v>FF</v>
+      </c>
+      <c r="L63" t="str">
+        <v>FF</v>
+      </c>
+      <c r="M63" t="str">
+        <v>FF</v>
+      </c>
+      <c r="N63" s="2" t="str">
+        <v>81</v>
+      </c>
+      <c r="O63" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="P63" s="1" t="str">
+        <v>00</v>
+      </c>
+      <c r="Q63" s="1" t="str">
+        <v>82</v>
+      </c>
+      <c r="R63" t="str">
+        <v>A5</v>
+      </c>
+      <c r="S63" t="str">
+        <v>03</v>
+      </c>
+      <c r="T63" t="str">
+        <v>00</v>
+      </c>
+      <c r="U63" t="str">
+        <v>0F</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F70))</f>
+        <v>AAFD02522070</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="F70" t="str" cm="1">
+        <f t="array" ref="F70:K70">TRANSPOSE(SUBSTITUTE(B65:B70,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G70" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H70" t="str">
+        <v>02</v>
+      </c>
+      <c r="I70" t="str">
+        <v>52</v>
+      </c>
+      <c r="J70" t="str">
+        <v>20</v>
+      </c>
+      <c r="K70" t="str">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C72" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C73" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C74" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C75" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C76" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C77" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C78" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F78" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F79))</f>
+        <v>AAFD03A01802B9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E79" s="2"/>
+      <c r="F79" t="str" cm="1">
+        <f t="array" ref="F79:L79">TRANSPOSE(SUBSTITUTE(C72:C78,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G79" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H79" t="str">
+        <v>03</v>
+      </c>
+      <c r="I79" t="str">
+        <v>A0</v>
+      </c>
+      <c r="J79" t="str">
+        <v>18</v>
+      </c>
+      <c r="K79" t="str">
+        <v>02</v>
+      </c>
+      <c r="L79" t="str">
+        <v>B9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="161" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B161" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="162" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B162" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="163" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B163" s="12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="164" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B164" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B165" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B166" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B167" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="168" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B168" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="169" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B169" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="170" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B170" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B171" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B172" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B173" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B174" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F174" t="str">
+        <f>_xlfn.CONCAT(_xlfn.ANCHORARRAY(F175))</f>
+        <v>AAFD0341FF41FCAAFD02034342AAFD0602400020203175AAFD090140003253494D505825AAFD080440000080000008C4AAFD02030302AAFD0203C3C2AAFD0602C100334850EEAAFD0901C000203133315620ADAAFD0225C1E6AAFD02038382</v>
+      </c>
+    </row>
+    <row r="175" spans="2:100" x14ac:dyDescent="0.25">
+      <c r="B175" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F175" t="str" cm="1">
+        <f t="array" ref="F175:CV175">TRANSPOSE(SUBSTITUTE(B81:B175,"0x",""))</f>
+        <v>AA</v>
+      </c>
+      <c r="G175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="H175" t="str">
+        <v>03</v>
+      </c>
+      <c r="I175" t="str">
+        <v>41</v>
+      </c>
+      <c r="J175" t="str">
+        <v>FF</v>
+      </c>
+      <c r="K175" t="str">
+        <v>41</v>
+      </c>
+      <c r="L175" t="str">
+        <v>FC</v>
+      </c>
+      <c r="M175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="N175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="O175" t="str">
+        <v>02</v>
+      </c>
+      <c r="P175" t="str">
+        <v>03</v>
+      </c>
+      <c r="Q175" t="str">
+        <v>43</v>
+      </c>
+      <c r="R175" t="str">
+        <v>42</v>
+      </c>
+      <c r="S175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="T175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="U175" t="str">
+        <v>06</v>
+      </c>
+      <c r="V175" t="str">
+        <v>02</v>
+      </c>
+      <c r="W175" t="str">
+        <v>40</v>
+      </c>
+      <c r="X175" t="str">
+        <v>00</v>
+      </c>
+      <c r="Y175" t="str">
+        <v>20</v>
+      </c>
+      <c r="Z175" t="str">
+        <v>20</v>
+      </c>
+      <c r="AA175" t="str">
+        <v>31</v>
+      </c>
+      <c r="AB175" t="str">
+        <v>75</v>
+      </c>
+      <c r="AC175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="AD175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="AE175" t="str">
+        <v>09</v>
+      </c>
+      <c r="AF175" t="str">
+        <v>01</v>
+      </c>
+      <c r="AG175" t="str">
+        <v>40</v>
+      </c>
+      <c r="AH175" t="str">
+        <v>00</v>
+      </c>
+      <c r="AI175" t="str">
+        <v>32</v>
+      </c>
+      <c r="AJ175" t="str">
+        <v>53</v>
+      </c>
+      <c r="AK175" t="str">
+        <v>49</v>
+      </c>
+      <c r="AL175" t="str">
+        <v>4D</v>
+      </c>
+      <c r="AM175" t="str">
+        <v>50</v>
+      </c>
+      <c r="AN175" t="str">
+        <v>58</v>
+      </c>
+      <c r="AO175" t="str">
+        <v>25</v>
+      </c>
+      <c r="AP175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="AQ175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="AR175" t="str">
+        <v>08</v>
+      </c>
+      <c r="AS175" t="str">
+        <v>04</v>
+      </c>
+      <c r="AT175" t="str">
+        <v>40</v>
+      </c>
+      <c r="AU175" t="str">
+        <v>00</v>
+      </c>
+      <c r="AV175" t="str">
+        <v>00</v>
+      </c>
+      <c r="AW175" t="str">
+        <v>80</v>
+      </c>
+      <c r="AX175" t="str">
+        <v>00</v>
+      </c>
+      <c r="AY175" t="str">
+        <v>00</v>
+      </c>
+      <c r="AZ175" t="str">
+        <v>08</v>
+      </c>
+      <c r="BA175" t="str">
+        <v>C4</v>
+      </c>
+      <c r="BB175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="BC175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="BD175" t="str">
+        <v>02</v>
+      </c>
+      <c r="BE175" t="str">
+        <v>03</v>
+      </c>
+      <c r="BF175" t="str">
+        <v>03</v>
+      </c>
+      <c r="BG175" t="str">
+        <v>02</v>
+      </c>
+      <c r="BH175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="BI175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="BJ175" t="str">
+        <v>02</v>
+      </c>
+      <c r="BK175" t="str">
+        <v>03</v>
+      </c>
+      <c r="BL175" t="str">
+        <v>C3</v>
+      </c>
+      <c r="BM175" t="str">
+        <v>C2</v>
+      </c>
+      <c r="BN175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="BO175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="BP175" t="str">
+        <v>06</v>
+      </c>
+      <c r="BQ175" t="str">
+        <v>02</v>
+      </c>
+      <c r="BR175" t="str">
+        <v>C1</v>
+      </c>
+      <c r="BS175" t="str">
+        <v>00</v>
+      </c>
+      <c r="BT175" t="str">
+        <v>33</v>
+      </c>
+      <c r="BU175" t="str">
+        <v>48</v>
+      </c>
+      <c r="BV175" t="str">
+        <v>50</v>
+      </c>
+      <c r="BW175" t="str">
+        <v>EE</v>
+      </c>
+      <c r="BX175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="BY175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="BZ175" t="str">
+        <v>09</v>
+      </c>
+      <c r="CA175" t="str">
+        <v>01</v>
+      </c>
+      <c r="CB175" t="str">
+        <v>C0</v>
+      </c>
+      <c r="CC175" t="str">
+        <v>00</v>
+      </c>
+      <c r="CD175" t="str">
+        <v>20</v>
+      </c>
+      <c r="CE175" t="str">
+        <v>31</v>
+      </c>
+      <c r="CF175" t="str">
+        <v>33</v>
+      </c>
+      <c r="CG175" t="str">
+        <v>31</v>
+      </c>
+      <c r="CH175" t="str">
+        <v>56</v>
+      </c>
+      <c r="CI175" t="str">
+        <v>20</v>
+      </c>
+      <c r="CJ175" t="str">
+        <v>AD</v>
+      </c>
+      <c r="CK175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="CL175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="CM175" t="str">
+        <v>02</v>
+      </c>
+      <c r="CN175" t="str">
+        <v>25</v>
+      </c>
+      <c r="CO175" t="str">
+        <v>C1</v>
+      </c>
+      <c r="CP175" t="str">
+        <v>E6</v>
+      </c>
+      <c r="CQ175" t="str">
+        <v>AA</v>
+      </c>
+      <c r="CR175" t="str">
+        <v>FD</v>
+      </c>
+      <c r="CS175" t="str">
+        <v>02</v>
+      </c>
+      <c r="CT175" t="str">
+        <v>03</v>
+      </c>
+      <c r="CU175" t="str">
+        <v>83</v>
+      </c>
+      <c r="CV175" t="str">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:DD1048576">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+      <formula>"AA"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+      <formula>"FD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+      <formula>"0xFD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+      <formula>"0xAA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899E6AC2-02D2-4A93-BEDF-BF379E35DB7E}">
   <dimension ref="A1:CE100"/>
   <sheetViews>
-    <sheetView topLeftCell="AF10" workbookViewId="0">
-      <selection activeCell="AP29" sqref="AP29"/>
+    <sheetView topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="BN8" sqref="BN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24348,7 +24144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB3AAAF-6AEC-4994-B7AA-E6FC07769F3A}">
   <dimension ref="B2:B4"/>
   <sheetViews>
@@ -24376,12 +24172,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A0B156-B528-431C-B24E-1CA04DF6378E}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="I51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q71" sqref="Q71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24440,7 +24236,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="20" t="s">
         <v>517</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -24647,7 +24443,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
-      <c r="Q7" s="52" t="s">
+      <c r="Q7" s="46" t="s">
         <v>403</v>
       </c>
     </row>
@@ -24770,7 +24566,7 @@
         <v>364</v>
       </c>
       <c r="M10" s="19"/>
-      <c r="Q10" s="52" t="s">
+      <c r="Q10" s="46" t="s">
         <v>404</v>
       </c>
     </row>
@@ -24932,7 +24728,7 @@
         <v>364</v>
       </c>
       <c r="M14" s="19"/>
-      <c r="Q14" s="52" t="s">
+      <c r="Q14" s="46" t="s">
         <v>405</v>
       </c>
     </row>
@@ -24974,7 +24770,7 @@
         <v>364</v>
       </c>
       <c r="M15" s="19"/>
-      <c r="Q15" s="52"/>
+      <c r="Q15" s="46"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
@@ -25095,7 +24891,7 @@
         <v>364</v>
       </c>
       <c r="M18" s="19"/>
-      <c r="Q18" s="52" t="s">
+      <c r="Q18" s="46" t="s">
         <v>406</v>
       </c>
     </row>
@@ -25242,7 +25038,7 @@
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
-      <c r="Q22" s="52"/>
+      <c r="Q22" s="46"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
@@ -25324,7 +25120,7 @@
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
-      <c r="Q25" s="52"/>
+      <c r="Q25" s="46"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
@@ -25352,7 +25148,7 @@
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
-      <c r="Q26" s="52" t="s">
+      <c r="Q26" s="46" t="s">
         <v>397</v>
       </c>
     </row>
@@ -25382,7 +25178,7 @@
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
-      <c r="Q27" s="52" t="s">
+      <c r="Q27" s="46" t="s">
         <v>396</v>
       </c>
     </row>
@@ -25717,7 +25513,7 @@
       <c r="K39" s="19"/>
       <c r="L39" s="19"/>
       <c r="M39" s="19"/>
-      <c r="Q39" s="54"/>
+      <c r="Q39" s="48"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
@@ -25745,7 +25541,7 @@
       <c r="K40" s="19"/>
       <c r="L40" s="19"/>
       <c r="M40" s="19"/>
-      <c r="Q40" s="54"/>
+      <c r="Q40" s="48"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -25773,7 +25569,7 @@
       <c r="K41" s="19"/>
       <c r="L41" s="19"/>
       <c r="M41" s="19"/>
-      <c r="Q41" s="54"/>
+      <c r="Q41" s="48"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -25801,7 +25597,7 @@
       <c r="K42" s="19"/>
       <c r="L42" s="19"/>
       <c r="M42" s="19"/>
-      <c r="Q42" s="54"/>
+      <c r="Q42" s="48"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
@@ -25829,7 +25625,7 @@
       <c r="K43" s="19"/>
       <c r="L43" s="19"/>
       <c r="M43" s="19"/>
-      <c r="Q43" s="54"/>
+      <c r="Q43" s="48"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
@@ -25859,7 +25655,7 @@
       <c r="K44" s="19"/>
       <c r="L44" s="19"/>
       <c r="M44" s="19"/>
-      <c r="Q44" s="54"/>
+      <c r="Q44" s="48"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
@@ -25887,7 +25683,7 @@
       <c r="K45" s="19"/>
       <c r="L45" s="19"/>
       <c r="M45" s="19"/>
-      <c r="Q45" s="54"/>
+      <c r="Q45" s="48"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
@@ -25917,7 +25713,7 @@
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
       <c r="M46" s="19"/>
-      <c r="Q46" s="54"/>
+      <c r="Q46" s="48"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
@@ -25945,7 +25741,7 @@
       <c r="K47" s="19"/>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
-      <c r="Q47" s="54"/>
+      <c r="Q47" s="48"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
@@ -25973,7 +25769,7 @@
       <c r="K48" s="19"/>
       <c r="L48" s="19"/>
       <c r="M48" s="19"/>
-      <c r="Q48" s="54"/>
+      <c r="Q48" s="48"/>
     </row>
     <row r="49" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
@@ -26638,22 +26434,22 @@
       </c>
     </row>
     <row r="72" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q72" s="53" t="s">
+      <c r="Q72" s="47" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="Q74" s="52" t="s">
+      <c r="Q74" s="46" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="Q75" s="52" t="s">
+      <c r="Q75" s="46" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q78" s="63" t="s">
+      <c r="Q78" s="56" t="s">
         <v>500</v>
       </c>
     </row>
@@ -26689,7 +26485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643B3517-8437-4592-8BB0-EC2672EC4154}">
   <dimension ref="A1:DH63"/>
   <sheetViews>
@@ -26719,8 +26515,8 @@
       <c r="B1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="4" t="s">
         <v>291</v>
       </c>
@@ -26731,8 +26527,8 @@
         <v>209</v>
       </c>
       <c r="H1" s="4"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
       <c r="K1" s="4" t="s">
         <v>291</v>
       </c>
@@ -26745,8 +26541,8 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
       <c r="U1" s="4" t="s">
         <v>291</v>
       </c>
@@ -26762,8 +26558,8 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
       <c r="AH1" s="4" t="s">
         <v>291</v>
       </c>
@@ -26778,8 +26574,8 @@
       <c r="AO1" s="4"/>
       <c r="AP1" s="4"/>
       <c r="AQ1" s="4"/>
-      <c r="AR1" s="47"/>
-      <c r="AS1" s="47"/>
+      <c r="AR1" s="58"/>
+      <c r="AS1" s="58"/>
       <c r="AT1" s="4" t="s">
         <v>291</v>
       </c>
@@ -51476,12 +51272,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187985C7-07CA-43F3-B35D-778ACF736C60}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52849,12 +52645,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6890003-6BCB-43D4-B3CF-C1199841BA70}">
   <dimension ref="A1:AR59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52876,14 +52672,14 @@
       <c r="R1" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
       <c r="AE1" s="16" t="s">
         <v>239</v>
       </c>
@@ -55177,12 +54973,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89532B3-11EA-43FB-8C77-E51E3C9C7D72}">
   <dimension ref="A1:BM70"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG53" sqref="AG53"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AV26" sqref="AV26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55215,14 +55011,14 @@
       <c r="L1" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="N1" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
       <c r="Y1" s="16" t="s">
         <v>240</v>
       </c>
@@ -55645,29 +55441,29 @@
       </c>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="AA4" s="49" t="s">
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="AA4" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="49"/>
-      <c r="AE4" s="49"/>
-      <c r="AF4" s="49"/>
+      <c r="AB4" s="60"/>
+      <c r="AC4" s="60"/>
+      <c r="AD4" s="60"/>
+      <c r="AE4" s="60"/>
+      <c r="AF4" s="60"/>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -56066,11 +55862,11 @@
       </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="N8" s="49" t="s">
+      <c r="N8" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str" cm="1">
@@ -57715,4 +57511,209 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF9E3CD-2759-404F-9723-870EF2ECB184}">
+  <dimension ref="A1:Z12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="9.140625" style="20"/>
+    <col min="27" max="16384" width="9.140625" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>490</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>522</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>490</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q4" s="55" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>521</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>486</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>